<commit_message>
Update 26.1.2022. - reading and writing to excel file
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -2,25 +2,39 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6375" yWindow="-12675" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="all games" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="bet games" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
+    <font>
+      <name val="Calibri"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -37,12 +51,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -55,16 +84,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -137,7 +173,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -147,44 +183,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -211,14 +247,32 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -245,6 +299,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -256,166 +328,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -428,12 +476,274 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Team2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Hatay BSB</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Elazig IL Ozel Idare</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PAS Giannina</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Niki Leukados</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Zkk Art Basket</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Vojvodina Novi Sad</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Al Khor</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Qatar SC</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Al Samaheej</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Sitra</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Lokomotiv-Kuban KrasnodarRUS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>LietkabelisLTU</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Brose Bamberg</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>S.Oliver Wurzburg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CB Gran CanariaESP</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Promitheas PatrasGRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Los Angeles Clippers</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Orlando Magic</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Milwaukee Bucks</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Cleveland Cavaliers</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>New York Knicks</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Miami Heat</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Sacramento Kings</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Atlanta Hawks</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Memphis Grizzlies</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>San Antonio Spurs</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Dallas Mavericks</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Phoenix Suns</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Utah Jazz</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="33" customWidth="1" style="3" min="2" max="2"/>
+    <col width="28.140625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="9.140625" customWidth="1" style="3" min="6" max="6"/>
+    <col width="12.85546875" customWidth="1" style="3" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Team1</t>
@@ -442,6 +752,26 @@
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Team2</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Bet team</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Spread</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Bet size</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Border score</t>
         </is>
       </c>
     </row>
@@ -451,13 +781,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Basketball Lowen Braunschweig</t>
+          <t>Hatay BSB</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>EWE Baskets Oldenburg</t>
-        </is>
+          <t>Elazig IL Ozel Idare</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="3">
@@ -466,13 +808,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ratiopharm UlmGER</t>
+          <t>PAS Giannina</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Virtus BolognaITA</t>
-        </is>
+          <t>Niki Leukados</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="4">
@@ -481,13 +835,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AZS UMCS LublinPOL</t>
+          <t>Zkk Art Basket</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Villeneuve D'AscqFRA</t>
-        </is>
+          <t>Vojvodina Novi Sad</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -496,13 +862,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Slask WroclawPOL</t>
+          <t>Al Khor</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Levallois MetropolitansFRA</t>
-        </is>
+          <t>Qatar SC</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="6">
@@ -511,13 +889,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Maccabi Tel AvivISR</t>
+          <t>Al Samaheej</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ALBA BerlinGER</t>
-        </is>
+          <t>Sitra</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="7">
@@ -526,13 +916,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Valencia BasketESP</t>
+          <t>Lokomotiv-Kuban KrasnodarRUS</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Buducnost VOLIMNE</t>
-        </is>
+          <t>LietkabelisLTU</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="8">
@@ -541,13 +943,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Real MadridESP</t>
+          <t>Brose Bamberg</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Unics KazanRUS</t>
-        </is>
+          <t>S.Oliver Wurzburg</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>5</v>
+      </c>
+      <c r="G8" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="9">
@@ -556,13 +970,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Asvel VilleurbanneFRA</t>
+          <t>CB Gran CanariaESP</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>FC Bayern MunichGER</t>
-        </is>
+          <t>Promitheas PatrasGRE</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F9" t="n">
+        <v>5</v>
+      </c>
+      <c r="G9" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="10">
@@ -571,13 +997,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Charlotte Hornets</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Toronto Raptors</t>
-        </is>
+          <t>Orlando Magic</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +1024,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Denver Nuggets</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Detroit Pistons</t>
-        </is>
+          <t>Cleveland Cavaliers</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G11" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="12">
@@ -601,13 +1051,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Los Angeles Clippers</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Washington Wizards</t>
-        </is>
+          <t>Miami Heat</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="13">
@@ -616,13 +1078,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>New Orleans Pelicans</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Philadelphia 76ers</t>
-        </is>
+          <t>Atlanta Hawks</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="14">
@@ -631,13 +1105,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Los Angeles Lakers</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Brooklyn Nets</t>
-        </is>
+          <t>San Antonio Spurs</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F14" t="n">
+        <v>5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="15">
@@ -646,13 +1132,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sacramento Kings</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Boston Celtics</t>
-        </is>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F15" t="n">
+        <v>5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="16">
@@ -661,16 +1159,29 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Dallas Mavericks</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Golden State Warriors</t>
-        </is>
+          <t>Utah Jazz</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>